<commit_message>
Modification Identified After Demo
</commit_message>
<xml_diff>
--- a/App_Templates/PackingList_Template.xlsx
+++ b/App_Templates/PackingList_Template.xlsx
@@ -14,14 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
-  <si>
-    <t>S.N.</t>
-  </si>
-  <si>
-    <t>Item 
-Code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Item Code</t>
   </si>
@@ -76,9 +69,6 @@
     <t>Height</t>
   </si>
   <si>
-    <t>ISGEC HEAVY ENGINEERING LTD.</t>
-  </si>
-  <si>
     <t>SERIAL NO</t>
   </si>
   <si>
@@ -116,13 +106,16 @@
   </si>
   <si>
     <t>GR DATE</t>
+  </si>
+  <si>
+    <t>ISGEC HEAVY ENGINEERING LTD. - PACKING LIST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,23 +150,29 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
+      <i/>
       <sz val="8"/>
       <color theme="4" tint="0.79998168889431442"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="8"/>
-      <color theme="4" tint="0.79998168889431442"/>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -472,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -499,47 +498,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -573,6 +548,33 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,25 +595,31 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>27216</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>585787</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>71438</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1089564</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>721176</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -619,20 +627,22 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="28575" y="371475"/>
-          <a:ext cx="1166812" cy="690563"/>
+          <a:off x="27216" y="27214"/>
+          <a:ext cx="1225634" cy="693962"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln w="1">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -930,291 +940,276 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="26.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="1.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="1.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="6" customWidth="1"/>
     <col min="4" max="4" width="26" style="6" customWidth="1"/>
     <col min="5" max="8" width="9.140625" style="5"/>
-    <col min="9" max="9" width="19.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="5" customWidth="1"/>
     <col min="10" max="10" width="27.5703125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" style="5" customWidth="1"/>
     <col min="12" max="12" width="13.140625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="11" style="5" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="5" customWidth="1"/>
     <col min="14" max="17" width="9.140625" style="5"/>
-    <col min="18" max="18" width="19.42578125" style="6" customWidth="1"/>
+    <col min="18" max="18" width="27.42578125" style="6" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="18"/>
+    <row r="1" spans="1:18" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="30"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="7"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="20"/>
+      <c r="K2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="32"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="7"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="20"/>
+      <c r="K3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="32"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="7"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="20"/>
+      <c r="K4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="32"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="7"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="20"/>
+      <c r="K5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="32"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
       <c r="I6" s="7"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="32"/>
+    </row>
+    <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="33"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="20"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="20"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="32"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="19"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="D9" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="E9" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="F9" s="23"/>
+      <c r="G9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="29" t="s">
+      <c r="K9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="24" t="s">
+      <c r="L9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="M9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="N9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="26" t="s">
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="24" t="s">
         <v>9</v>
-      </c>
-      <c r="N9" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="32" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="O10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="25"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="Q10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R10" s="33"/>
+        <v>10</v>
+      </c>
+      <c r="R10" s="25"/>
     </row>
   </sheetData>
   <sheetProtection password="CF0D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0"/>
   <mergeCells count="26">
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="J9:J10"/>
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="L2:R2"/>
@@ -1229,6 +1224,18 @@
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="J9:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>